<commit_message>
Documentacion nueva y actualizaciones
</commit_message>
<xml_diff>
--- a/PP-PMC/Plan de proyecto.xlsx
+++ b/PP-PMC/Plan de proyecto.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
   <si>
     <t>Reuniones con los demás departamentos</t>
   </si>
@@ -168,12 +168,18 @@
   <si>
     <t>%</t>
   </si>
+  <si>
+    <t>Esperado</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +245,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -284,7 +297,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -829,15 +842,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -845,28 +849,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -894,7 +876,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -981,8 +963,51 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="7" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1001,61 +1026,16 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="5" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="7" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="7" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="9" fillId="7" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1063,7 +1043,113 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1367,114 +1453,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AQ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CG40" sqref="CG40"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA45" sqref="AA45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="63.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="4" customWidth="1"/>
+    <col min="82" max="82" width="6.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
-      <c r="Z1" s="63"/>
-      <c r="AA1" s="63"/>
-      <c r="AB1" s="63"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="62" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="79"/>
+      <c r="AG1" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="63"/>
-      <c r="AJ1" s="63"/>
-      <c r="AK1" s="63"/>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="63"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="63"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="63"/>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="63"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="63"/>
-      <c r="BB1" s="63"/>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="63"/>
-      <c r="BE1" s="63"/>
-      <c r="BF1" s="63"/>
-      <c r="BG1" s="63"/>
-      <c r="BH1" s="63"/>
-      <c r="BI1" s="63"/>
-      <c r="BJ1" s="63"/>
-      <c r="BK1" s="64"/>
-      <c r="BL1" s="65" t="s">
+      <c r="AH1" s="78"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
+      <c r="AZ1" s="78"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="78"/>
+      <c r="BC1" s="78"/>
+      <c r="BD1" s="78"/>
+      <c r="BE1" s="78"/>
+      <c r="BF1" s="78"/>
+      <c r="BG1" s="78"/>
+      <c r="BH1" s="78"/>
+      <c r="BI1" s="78"/>
+      <c r="BJ1" s="78"/>
+      <c r="BK1" s="79"/>
+      <c r="BL1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="BM1" s="66"/>
-      <c r="BN1" s="66"/>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="66"/>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="66"/>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="67"/>
-      <c r="CC1" s="79" t="s">
+      <c r="BM1" s="81"/>
+      <c r="BN1" s="81"/>
+      <c r="BO1" s="81"/>
+      <c r="BP1" s="81"/>
+      <c r="BQ1" s="81"/>
+      <c r="BR1" s="81"/>
+      <c r="BS1" s="81"/>
+      <c r="BT1" s="81"/>
+      <c r="BU1" s="81"/>
+      <c r="BV1" s="81"/>
+      <c r="BW1" s="81"/>
+      <c r="BX1" s="81"/>
+      <c r="BY1" s="81"/>
+      <c r="BZ1" s="81"/>
+      <c r="CA1" s="81"/>
+      <c r="CB1" s="82"/>
+      <c r="CC1" s="70" t="s">
         <v>49</v>
       </c>
-      <c r="CD1" s="80"/>
+      <c r="CD1" s="71"/>
     </row>
     <row r="2" spans="1:82" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="69"/>
-      <c r="B2" s="75">
+      <c r="A2" s="65"/>
+      <c r="B2" s="62">
         <v>1</v>
       </c>
       <c r="C2" s="18">
@@ -1711,96 +1797,96 @@
       <c r="CB2" s="56">
         <v>17</v>
       </c>
-      <c r="CC2" s="81"/>
-      <c r="CD2" s="82"/>
+      <c r="CC2" s="68"/>
+      <c r="CD2" s="69"/>
     </row>
     <row r="3" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
-      <c r="O3" s="71"/>
-      <c r="P3" s="71"/>
-      <c r="Q3" s="71"/>
-      <c r="R3" s="71"/>
-      <c r="S3" s="71"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="71"/>
-      <c r="W3" s="71"/>
-      <c r="X3" s="71"/>
-      <c r="Y3" s="71"/>
-      <c r="Z3" s="71"/>
-      <c r="AA3" s="71"/>
-      <c r="AB3" s="71"/>
-      <c r="AC3" s="71"/>
-      <c r="AD3" s="71"/>
-      <c r="AE3" s="71"/>
-      <c r="AF3" s="71"/>
-      <c r="AG3" s="71"/>
-      <c r="AH3" s="71"/>
-      <c r="AI3" s="71"/>
-      <c r="AJ3" s="71"/>
-      <c r="AK3" s="71"/>
-      <c r="AL3" s="71"/>
-      <c r="AM3" s="71"/>
-      <c r="AN3" s="71"/>
-      <c r="AO3" s="71"/>
-      <c r="AP3" s="71"/>
-      <c r="AQ3" s="71"/>
-      <c r="AR3" s="71"/>
-      <c r="AS3" s="71"/>
-      <c r="AT3" s="71"/>
-      <c r="AU3" s="71"/>
-      <c r="AV3" s="71"/>
-      <c r="AW3" s="71"/>
-      <c r="AX3" s="71"/>
-      <c r="AY3" s="71"/>
-      <c r="AZ3" s="71"/>
-      <c r="BA3" s="71"/>
-      <c r="BB3" s="71"/>
-      <c r="BC3" s="71"/>
-      <c r="BD3" s="71"/>
-      <c r="BE3" s="71"/>
-      <c r="BF3" s="71"/>
-      <c r="BG3" s="71"/>
-      <c r="BH3" s="71"/>
-      <c r="BI3" s="71"/>
-      <c r="BJ3" s="71"/>
-      <c r="BK3" s="71"/>
-      <c r="BL3" s="71"/>
-      <c r="BM3" s="71"/>
-      <c r="BN3" s="71"/>
-      <c r="BO3" s="71"/>
-      <c r="BP3" s="71"/>
-      <c r="BQ3" s="71"/>
-      <c r="BR3" s="71"/>
-      <c r="BS3" s="71"/>
-      <c r="BT3" s="71"/>
-      <c r="BU3" s="71"/>
-      <c r="BV3" s="71"/>
-      <c r="BW3" s="71"/>
-      <c r="BX3" s="71"/>
-      <c r="BY3" s="71"/>
-      <c r="BZ3" s="71"/>
-      <c r="CA3" s="71"/>
-      <c r="CB3" s="71"/>
-      <c r="CC3" s="71"/>
-      <c r="CD3" s="72"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
+      <c r="U3" s="67"/>
+      <c r="V3" s="67"/>
+      <c r="W3" s="67"/>
+      <c r="X3" s="67"/>
+      <c r="Y3" s="67"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="67"/>
+      <c r="AE3" s="67"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="67"/>
+      <c r="AH3" s="67"/>
+      <c r="AI3" s="67"/>
+      <c r="AJ3" s="67"/>
+      <c r="AK3" s="67"/>
+      <c r="AL3" s="67"/>
+      <c r="AM3" s="67"/>
+      <c r="AN3" s="67"/>
+      <c r="AO3" s="67"/>
+      <c r="AP3" s="67"/>
+      <c r="AQ3" s="67"/>
+      <c r="AR3" s="67"/>
+      <c r="AS3" s="67"/>
+      <c r="AT3" s="67"/>
+      <c r="AU3" s="67"/>
+      <c r="AV3" s="67"/>
+      <c r="AW3" s="67"/>
+      <c r="AX3" s="67"/>
+      <c r="AY3" s="67"/>
+      <c r="AZ3" s="67"/>
+      <c r="BA3" s="67"/>
+      <c r="BB3" s="67"/>
+      <c r="BC3" s="67"/>
+      <c r="BD3" s="67"/>
+      <c r="BE3" s="67"/>
+      <c r="BF3" s="67"/>
+      <c r="BG3" s="67"/>
+      <c r="BH3" s="67"/>
+      <c r="BI3" s="67"/>
+      <c r="BJ3" s="67"/>
+      <c r="BK3" s="67"/>
+      <c r="BL3" s="67"/>
+      <c r="BM3" s="67"/>
+      <c r="BN3" s="67"/>
+      <c r="BO3" s="67"/>
+      <c r="BP3" s="67"/>
+      <c r="BQ3" s="67"/>
+      <c r="BR3" s="67"/>
+      <c r="BS3" s="67"/>
+      <c r="BT3" s="67"/>
+      <c r="BU3" s="67"/>
+      <c r="BV3" s="67"/>
+      <c r="BW3" s="67"/>
+      <c r="BX3" s="67"/>
+      <c r="BY3" s="67"/>
+      <c r="BZ3" s="67"/>
+      <c r="CA3" s="67"/>
+      <c r="CB3" s="67"/>
+      <c r="CC3" s="67"/>
+      <c r="CD3" s="76"/>
     </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="21" t="s">
         <v>30</v>
       </c>
@@ -1883,10 +1969,10 @@
       <c r="BZ4" s="6"/>
       <c r="CA4" s="6"/>
       <c r="CB4" s="57"/>
-      <c r="CC4" s="83">
-        <v>0.4</v>
-      </c>
-      <c r="CD4" s="84"/>
+      <c r="CC4" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="CD4" s="86"/>
     </row>
     <row r="5" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
@@ -1971,10 +2057,12 @@
       <c r="BZ5" s="6"/>
       <c r="CA5" s="6"/>
       <c r="CB5" s="57"/>
-      <c r="CC5" s="85"/>
-      <c r="CD5" s="86"/>
+      <c r="CC5" s="72">
+        <v>0.4</v>
+      </c>
+      <c r="CD5" s="73"/>
     </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>27</v>
       </c>
@@ -2057,10 +2145,10 @@
       <c r="BZ6" s="2"/>
       <c r="CA6" s="2"/>
       <c r="CB6" s="58"/>
-      <c r="CC6" s="85"/>
-      <c r="CD6" s="86"/>
+      <c r="CC6" s="72"/>
+      <c r="CD6" s="73"/>
     </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>28</v>
       </c>
@@ -2143,7 +2231,9 @@
       <c r="BZ7" s="2"/>
       <c r="CA7" s="2"/>
       <c r="CB7" s="58"/>
-      <c r="CC7" s="85"/>
+      <c r="CC7" s="85" t="s">
+        <v>50</v>
+      </c>
       <c r="CD7" s="86"/>
     </row>
     <row r="8" spans="1:82" x14ac:dyDescent="0.3">
@@ -2229,8 +2319,10 @@
       <c r="BZ8" s="2"/>
       <c r="CA8" s="2"/>
       <c r="CB8" s="58"/>
-      <c r="CC8" s="85"/>
-      <c r="CD8" s="86"/>
+      <c r="CC8" s="72">
+        <v>0.5</v>
+      </c>
+      <c r="CD8" s="73"/>
     </row>
     <row r="9" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
@@ -2315,8 +2407,8 @@
       <c r="BZ9" s="37"/>
       <c r="CA9" s="37"/>
       <c r="CB9" s="55"/>
-      <c r="CC9" s="85"/>
-      <c r="CD9" s="86"/>
+      <c r="CC9" s="72"/>
+      <c r="CD9" s="73"/>
     </row>
     <row r="10" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
@@ -2401,96 +2493,96 @@
       <c r="BZ10" s="37"/>
       <c r="CA10" s="37"/>
       <c r="CB10" s="55"/>
-      <c r="CC10" s="87"/>
-      <c r="CD10" s="88"/>
+      <c r="CC10" s="74"/>
+      <c r="CD10" s="75"/>
     </row>
     <row r="11" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="70"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="71"/>
-      <c r="P11" s="71"/>
-      <c r="Q11" s="71"/>
-      <c r="R11" s="71"/>
-      <c r="S11" s="71"/>
-      <c r="T11" s="71"/>
-      <c r="U11" s="71"/>
-      <c r="V11" s="71"/>
-      <c r="W11" s="71"/>
-      <c r="X11" s="71"/>
-      <c r="Y11" s="71"/>
-      <c r="Z11" s="71"/>
-      <c r="AA11" s="71"/>
-      <c r="AB11" s="71"/>
-      <c r="AC11" s="71"/>
-      <c r="AD11" s="71"/>
-      <c r="AE11" s="71"/>
-      <c r="AF11" s="71"/>
-      <c r="AG11" s="71"/>
-      <c r="AH11" s="71"/>
-      <c r="AI11" s="71"/>
-      <c r="AJ11" s="71"/>
-      <c r="AK11" s="71"/>
-      <c r="AL11" s="71"/>
-      <c r="AM11" s="71"/>
-      <c r="AN11" s="71"/>
-      <c r="AO11" s="71"/>
-      <c r="AP11" s="71"/>
-      <c r="AQ11" s="71"/>
-      <c r="AR11" s="71"/>
-      <c r="AS11" s="71"/>
-      <c r="AT11" s="71"/>
-      <c r="AU11" s="71"/>
-      <c r="AV11" s="71"/>
-      <c r="AW11" s="71"/>
-      <c r="AX11" s="71"/>
-      <c r="AY11" s="71"/>
-      <c r="AZ11" s="71"/>
-      <c r="BA11" s="71"/>
-      <c r="BB11" s="71"/>
-      <c r="BC11" s="71"/>
-      <c r="BD11" s="71"/>
-      <c r="BE11" s="71"/>
-      <c r="BF11" s="71"/>
-      <c r="BG11" s="71"/>
-      <c r="BH11" s="71"/>
-      <c r="BI11" s="71"/>
-      <c r="BJ11" s="71"/>
-      <c r="BK11" s="71"/>
-      <c r="BL11" s="71"/>
-      <c r="BM11" s="71"/>
-      <c r="BN11" s="71"/>
-      <c r="BO11" s="71"/>
-      <c r="BP11" s="71"/>
-      <c r="BQ11" s="71"/>
-      <c r="BR11" s="71"/>
-      <c r="BS11" s="71"/>
-      <c r="BT11" s="71"/>
-      <c r="BU11" s="71"/>
-      <c r="BV11" s="71"/>
-      <c r="BW11" s="71"/>
-      <c r="BX11" s="71"/>
-      <c r="BY11" s="71"/>
-      <c r="BZ11" s="71"/>
-      <c r="CA11" s="71"/>
-      <c r="CB11" s="71"/>
-      <c r="CC11" s="77"/>
-      <c r="CD11" s="78"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
+      <c r="Q11" s="67"/>
+      <c r="R11" s="67"/>
+      <c r="S11" s="67"/>
+      <c r="T11" s="67"/>
+      <c r="U11" s="67"/>
+      <c r="V11" s="67"/>
+      <c r="W11" s="67"/>
+      <c r="X11" s="67"/>
+      <c r="Y11" s="67"/>
+      <c r="Z11" s="67"/>
+      <c r="AA11" s="67"/>
+      <c r="AB11" s="67"/>
+      <c r="AC11" s="67"/>
+      <c r="AD11" s="67"/>
+      <c r="AE11" s="67"/>
+      <c r="AF11" s="67"/>
+      <c r="AG11" s="67"/>
+      <c r="AH11" s="67"/>
+      <c r="AI11" s="67"/>
+      <c r="AJ11" s="67"/>
+      <c r="AK11" s="67"/>
+      <c r="AL11" s="67"/>
+      <c r="AM11" s="67"/>
+      <c r="AN11" s="67"/>
+      <c r="AO11" s="67"/>
+      <c r="AP11" s="67"/>
+      <c r="AQ11" s="67"/>
+      <c r="AR11" s="67"/>
+      <c r="AS11" s="67"/>
+      <c r="AT11" s="67"/>
+      <c r="AU11" s="67"/>
+      <c r="AV11" s="67"/>
+      <c r="AW11" s="67"/>
+      <c r="AX11" s="67"/>
+      <c r="AY11" s="67"/>
+      <c r="AZ11" s="67"/>
+      <c r="BA11" s="67"/>
+      <c r="BB11" s="67"/>
+      <c r="BC11" s="67"/>
+      <c r="BD11" s="67"/>
+      <c r="BE11" s="67"/>
+      <c r="BF11" s="67"/>
+      <c r="BG11" s="67"/>
+      <c r="BH11" s="67"/>
+      <c r="BI11" s="67"/>
+      <c r="BJ11" s="67"/>
+      <c r="BK11" s="67"/>
+      <c r="BL11" s="67"/>
+      <c r="BM11" s="67"/>
+      <c r="BN11" s="67"/>
+      <c r="BO11" s="67"/>
+      <c r="BP11" s="67"/>
+      <c r="BQ11" s="67"/>
+      <c r="BR11" s="67"/>
+      <c r="BS11" s="67"/>
+      <c r="BT11" s="67"/>
+      <c r="BU11" s="67"/>
+      <c r="BV11" s="67"/>
+      <c r="BW11" s="67"/>
+      <c r="BX11" s="67"/>
+      <c r="BY11" s="67"/>
+      <c r="BZ11" s="67"/>
+      <c r="CA11" s="67"/>
+      <c r="CB11" s="67"/>
+      <c r="CC11" s="83"/>
+      <c r="CD11" s="84"/>
     </row>
-    <row r="12" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="24" t="s">
         <v>0</v>
       </c>
@@ -2533,28 +2625,28 @@
       <c r="AL12" s="6"/>
       <c r="AM12" s="6"/>
       <c r="AN12" s="6"/>
-      <c r="AO12" s="74"/>
+      <c r="AO12" s="61"/>
       <c r="AP12" s="6"/>
       <c r="AQ12" s="6"/>
       <c r="AR12" s="6"/>
       <c r="AS12" s="6"/>
       <c r="AT12" s="6"/>
       <c r="AU12" s="6"/>
-      <c r="AV12" s="74"/>
+      <c r="AV12" s="61"/>
       <c r="AW12" s="6"/>
       <c r="AX12" s="6"/>
       <c r="AY12" s="6"/>
       <c r="AZ12" s="6"/>
       <c r="BA12" s="6"/>
       <c r="BB12" s="6"/>
-      <c r="BC12" s="74"/>
+      <c r="BC12" s="61"/>
       <c r="BD12" s="6"/>
       <c r="BE12" s="6"/>
       <c r="BF12" s="6"/>
       <c r="BG12" s="6"/>
       <c r="BH12" s="6"/>
       <c r="BI12" s="6"/>
-      <c r="BJ12" s="74"/>
+      <c r="BJ12" s="61"/>
       <c r="BK12" s="7"/>
       <c r="BL12" s="32"/>
       <c r="BM12" s="6"/>
@@ -2573,10 +2665,10 @@
       <c r="BZ12" s="6"/>
       <c r="CA12" s="6"/>
       <c r="CB12" s="57"/>
-      <c r="CC12" s="83">
-        <v>0.6</v>
-      </c>
-      <c r="CD12" s="84"/>
+      <c r="CC12" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="CD12" s="86"/>
     </row>
     <row r="13" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -2661,8 +2753,10 @@
       <c r="BZ13" s="2"/>
       <c r="CA13" s="2"/>
       <c r="CB13" s="58"/>
-      <c r="CC13" s="85"/>
-      <c r="CD13" s="86"/>
+      <c r="CC13" s="72">
+        <v>0.6</v>
+      </c>
+      <c r="CD13" s="73"/>
     </row>
     <row r="14" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -2747,10 +2841,10 @@
       <c r="BZ14" s="2"/>
       <c r="CA14" s="2"/>
       <c r="CB14" s="58"/>
-      <c r="CC14" s="85"/>
-      <c r="CD14" s="86"/>
+      <c r="CC14" s="72"/>
+      <c r="CD14" s="73"/>
     </row>
-    <row r="15" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
         <v>3</v>
       </c>
@@ -2833,10 +2927,10 @@
       <c r="BZ15" s="2"/>
       <c r="CA15" s="2"/>
       <c r="CB15" s="58"/>
-      <c r="CC15" s="85"/>
-      <c r="CD15" s="86"/>
+      <c r="CC15" s="72"/>
+      <c r="CD15" s="73"/>
     </row>
-    <row r="16" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="24" t="s">
         <v>4</v>
       </c>
@@ -2919,7 +3013,9 @@
       <c r="BZ16" s="2"/>
       <c r="CA16" s="2"/>
       <c r="CB16" s="58"/>
-      <c r="CC16" s="85"/>
+      <c r="CC16" s="85" t="s">
+        <v>50</v>
+      </c>
       <c r="CD16" s="86"/>
     </row>
     <row r="17" spans="1:82" x14ac:dyDescent="0.3">
@@ -3005,8 +3101,10 @@
       <c r="BZ17" s="2"/>
       <c r="CA17" s="2"/>
       <c r="CB17" s="58"/>
-      <c r="CC17" s="85"/>
-      <c r="CD17" s="86"/>
+      <c r="CC17" s="72">
+        <v>0.6</v>
+      </c>
+      <c r="CD17" s="73"/>
     </row>
     <row r="18" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
@@ -3091,8 +3189,8 @@
       <c r="BZ18" s="2"/>
       <c r="CA18" s="2"/>
       <c r="CB18" s="58"/>
-      <c r="CC18" s="85"/>
-      <c r="CD18" s="86"/>
+      <c r="CC18" s="72"/>
+      <c r="CD18" s="73"/>
     </row>
     <row r="19" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
@@ -3177,8 +3275,8 @@
       <c r="BZ19" s="2"/>
       <c r="CA19" s="2"/>
       <c r="CB19" s="58"/>
-      <c r="CC19" s="85"/>
-      <c r="CD19" s="86"/>
+      <c r="CC19" s="72"/>
+      <c r="CD19" s="73"/>
     </row>
     <row r="20" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
@@ -3214,7 +3312,7 @@
       <c r="AC20" s="47"/>
       <c r="AD20" s="47"/>
       <c r="AE20" s="47"/>
-      <c r="AF20" s="76"/>
+      <c r="AF20" s="63"/>
       <c r="AG20" s="47"/>
       <c r="AH20" s="47"/>
       <c r="AI20" s="38"/>
@@ -3263,96 +3361,96 @@
       <c r="BZ20" s="37"/>
       <c r="CA20" s="37"/>
       <c r="CB20" s="55"/>
-      <c r="CC20" s="87"/>
-      <c r="CD20" s="88"/>
+      <c r="CC20" s="74"/>
+      <c r="CD20" s="75"/>
     </row>
     <row r="21" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="70"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="71"/>
-      <c r="N21" s="71"/>
-      <c r="O21" s="71"/>
-      <c r="P21" s="71"/>
-      <c r="Q21" s="71"/>
-      <c r="R21" s="71"/>
-      <c r="S21" s="71"/>
-      <c r="T21" s="71"/>
-      <c r="U21" s="71"/>
-      <c r="V21" s="71"/>
-      <c r="W21" s="71"/>
-      <c r="X21" s="71"/>
-      <c r="Y21" s="71"/>
-      <c r="Z21" s="71"/>
-      <c r="AA21" s="71"/>
-      <c r="AB21" s="71"/>
-      <c r="AC21" s="71"/>
-      <c r="AD21" s="71"/>
-      <c r="AE21" s="71"/>
-      <c r="AF21" s="71"/>
-      <c r="AG21" s="71"/>
-      <c r="AH21" s="71"/>
-      <c r="AI21" s="71"/>
-      <c r="AJ21" s="71"/>
-      <c r="AK21" s="71"/>
-      <c r="AL21" s="71"/>
-      <c r="AM21" s="71"/>
-      <c r="AN21" s="71"/>
-      <c r="AO21" s="71"/>
-      <c r="AP21" s="71"/>
-      <c r="AQ21" s="71"/>
-      <c r="AR21" s="71"/>
-      <c r="AS21" s="71"/>
-      <c r="AT21" s="71"/>
-      <c r="AU21" s="71"/>
-      <c r="AV21" s="71"/>
-      <c r="AW21" s="71"/>
-      <c r="AX21" s="71"/>
-      <c r="AY21" s="71"/>
-      <c r="AZ21" s="71"/>
-      <c r="BA21" s="71"/>
-      <c r="BB21" s="71"/>
-      <c r="BC21" s="71"/>
-      <c r="BD21" s="71"/>
-      <c r="BE21" s="71"/>
-      <c r="BF21" s="71"/>
-      <c r="BG21" s="71"/>
-      <c r="BH21" s="71"/>
-      <c r="BI21" s="71"/>
-      <c r="BJ21" s="71"/>
-      <c r="BK21" s="71"/>
-      <c r="BL21" s="71"/>
-      <c r="BM21" s="71"/>
-      <c r="BN21" s="71"/>
-      <c r="BO21" s="71"/>
-      <c r="BP21" s="71"/>
-      <c r="BQ21" s="71"/>
-      <c r="BR21" s="71"/>
-      <c r="BS21" s="71"/>
-      <c r="BT21" s="71"/>
-      <c r="BU21" s="71"/>
-      <c r="BV21" s="71"/>
-      <c r="BW21" s="71"/>
-      <c r="BX21" s="71"/>
-      <c r="BY21" s="71"/>
-      <c r="BZ21" s="71"/>
-      <c r="CA21" s="71"/>
-      <c r="CB21" s="71"/>
-      <c r="CC21" s="77"/>
-      <c r="CD21" s="78"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
+      <c r="N21" s="67"/>
+      <c r="O21" s="67"/>
+      <c r="P21" s="67"/>
+      <c r="Q21" s="67"/>
+      <c r="R21" s="67"/>
+      <c r="S21" s="67"/>
+      <c r="T21" s="67"/>
+      <c r="U21" s="67"/>
+      <c r="V21" s="67"/>
+      <c r="W21" s="67"/>
+      <c r="X21" s="67"/>
+      <c r="Y21" s="67"/>
+      <c r="Z21" s="67"/>
+      <c r="AA21" s="67"/>
+      <c r="AB21" s="67"/>
+      <c r="AC21" s="67"/>
+      <c r="AD21" s="67"/>
+      <c r="AE21" s="67"/>
+      <c r="AF21" s="67"/>
+      <c r="AG21" s="67"/>
+      <c r="AH21" s="67"/>
+      <c r="AI21" s="67"/>
+      <c r="AJ21" s="67"/>
+      <c r="AK21" s="67"/>
+      <c r="AL21" s="67"/>
+      <c r="AM21" s="67"/>
+      <c r="AN21" s="67"/>
+      <c r="AO21" s="67"/>
+      <c r="AP21" s="67"/>
+      <c r="AQ21" s="67"/>
+      <c r="AR21" s="67"/>
+      <c r="AS21" s="67"/>
+      <c r="AT21" s="67"/>
+      <c r="AU21" s="67"/>
+      <c r="AV21" s="67"/>
+      <c r="AW21" s="67"/>
+      <c r="AX21" s="67"/>
+      <c r="AY21" s="67"/>
+      <c r="AZ21" s="67"/>
+      <c r="BA21" s="67"/>
+      <c r="BB21" s="67"/>
+      <c r="BC21" s="67"/>
+      <c r="BD21" s="67"/>
+      <c r="BE21" s="67"/>
+      <c r="BF21" s="67"/>
+      <c r="BG21" s="67"/>
+      <c r="BH21" s="67"/>
+      <c r="BI21" s="67"/>
+      <c r="BJ21" s="67"/>
+      <c r="BK21" s="67"/>
+      <c r="BL21" s="67"/>
+      <c r="BM21" s="67"/>
+      <c r="BN21" s="67"/>
+      <c r="BO21" s="67"/>
+      <c r="BP21" s="67"/>
+      <c r="BQ21" s="67"/>
+      <c r="BR21" s="67"/>
+      <c r="BS21" s="67"/>
+      <c r="BT21" s="67"/>
+      <c r="BU21" s="67"/>
+      <c r="BV21" s="67"/>
+      <c r="BW21" s="67"/>
+      <c r="BX21" s="67"/>
+      <c r="BY21" s="67"/>
+      <c r="BZ21" s="67"/>
+      <c r="CA21" s="67"/>
+      <c r="CB21" s="67"/>
+      <c r="CC21" s="83"/>
+      <c r="CD21" s="84"/>
     </row>
-    <row r="22" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="26" t="s">
         <v>16</v>
       </c>
@@ -3435,10 +3533,10 @@
       <c r="BZ22" s="6"/>
       <c r="CA22" s="6"/>
       <c r="CB22" s="57"/>
-      <c r="CC22" s="83">
-        <v>0.3</v>
-      </c>
-      <c r="CD22" s="84"/>
+      <c r="CC22" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="CD22" s="86"/>
     </row>
     <row r="23" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
@@ -3523,8 +3621,10 @@
       <c r="BZ23" s="2"/>
       <c r="CA23" s="2"/>
       <c r="CB23" s="58"/>
-      <c r="CC23" s="85"/>
-      <c r="CD23" s="86"/>
+      <c r="CC23" s="72">
+        <v>0.3</v>
+      </c>
+      <c r="CD23" s="73"/>
     </row>
     <row r="24" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
@@ -3609,10 +3709,10 @@
       <c r="BZ24" s="2"/>
       <c r="CA24" s="2"/>
       <c r="CB24" s="58"/>
-      <c r="CC24" s="85"/>
-      <c r="CD24" s="86"/>
+      <c r="CC24" s="72"/>
+      <c r="CD24" s="73"/>
     </row>
-    <row r="25" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>19</v>
       </c>
@@ -3695,10 +3795,10 @@
       <c r="BZ25" s="2"/>
       <c r="CA25" s="2"/>
       <c r="CB25" s="58"/>
-      <c r="CC25" s="85"/>
-      <c r="CD25" s="86"/>
+      <c r="CC25" s="72"/>
+      <c r="CD25" s="73"/>
     </row>
-    <row r="26" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>20</v>
       </c>
@@ -3781,7 +3881,9 @@
       <c r="BZ26" s="2"/>
       <c r="CA26" s="2"/>
       <c r="CB26" s="58"/>
-      <c r="CC26" s="85"/>
+      <c r="CC26" s="85" t="s">
+        <v>50</v>
+      </c>
       <c r="CD26" s="86"/>
     </row>
     <row r="27" spans="1:82" x14ac:dyDescent="0.3">
@@ -3867,8 +3969,10 @@
       <c r="BZ27" s="2"/>
       <c r="CA27" s="2"/>
       <c r="CB27" s="58"/>
-      <c r="CC27" s="85"/>
-      <c r="CD27" s="86"/>
+      <c r="CC27" s="72">
+        <v>0.4</v>
+      </c>
+      <c r="CD27" s="73"/>
     </row>
     <row r="28" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
@@ -3953,8 +4057,8 @@
       <c r="BZ28" s="2"/>
       <c r="CA28" s="2"/>
       <c r="CB28" s="58"/>
-      <c r="CC28" s="85"/>
-      <c r="CD28" s="86"/>
+      <c r="CC28" s="72"/>
+      <c r="CD28" s="73"/>
     </row>
     <row r="29" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
@@ -4039,14 +4143,14 @@
       <c r="BZ29" s="2"/>
       <c r="CA29" s="2"/>
       <c r="CB29" s="58"/>
-      <c r="CC29" s="85"/>
-      <c r="CD29" s="86"/>
+      <c r="CC29" s="72"/>
+      <c r="CD29" s="73"/>
     </row>
     <row r="30" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="73"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="37"/>
       <c r="D30" s="37"/>
       <c r="E30" s="37"/>
@@ -4125,96 +4229,96 @@
       <c r="BZ30" s="37"/>
       <c r="CA30" s="37"/>
       <c r="CB30" s="55"/>
-      <c r="CC30" s="87"/>
-      <c r="CD30" s="88"/>
+      <c r="CC30" s="74"/>
+      <c r="CD30" s="75"/>
     </row>
     <row r="31" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="71"/>
-      <c r="L31" s="71"/>
-      <c r="M31" s="71"/>
-      <c r="N31" s="71"/>
-      <c r="O31" s="71"/>
-      <c r="P31" s="71"/>
-      <c r="Q31" s="71"/>
-      <c r="R31" s="71"/>
-      <c r="S31" s="71"/>
-      <c r="T31" s="71"/>
-      <c r="U31" s="71"/>
-      <c r="V31" s="71"/>
-      <c r="W31" s="71"/>
-      <c r="X31" s="71"/>
-      <c r="Y31" s="71"/>
-      <c r="Z31" s="71"/>
-      <c r="AA31" s="71"/>
-      <c r="AB31" s="71"/>
-      <c r="AC31" s="71"/>
-      <c r="AD31" s="71"/>
-      <c r="AE31" s="71"/>
-      <c r="AF31" s="71"/>
-      <c r="AG31" s="71"/>
-      <c r="AH31" s="71"/>
-      <c r="AI31" s="71"/>
-      <c r="AJ31" s="71"/>
-      <c r="AK31" s="71"/>
-      <c r="AL31" s="71"/>
-      <c r="AM31" s="71"/>
-      <c r="AN31" s="71"/>
-      <c r="AO31" s="71"/>
-      <c r="AP31" s="71"/>
-      <c r="AQ31" s="71"/>
-      <c r="AR31" s="71"/>
-      <c r="AS31" s="71"/>
-      <c r="AT31" s="71"/>
-      <c r="AU31" s="71"/>
-      <c r="AV31" s="71"/>
-      <c r="AW31" s="71"/>
-      <c r="AX31" s="71"/>
-      <c r="AY31" s="71"/>
-      <c r="AZ31" s="71"/>
-      <c r="BA31" s="71"/>
-      <c r="BB31" s="71"/>
-      <c r="BC31" s="71"/>
-      <c r="BD31" s="71"/>
-      <c r="BE31" s="71"/>
-      <c r="BF31" s="71"/>
-      <c r="BG31" s="71"/>
-      <c r="BH31" s="71"/>
-      <c r="BI31" s="71"/>
-      <c r="BJ31" s="71"/>
-      <c r="BK31" s="71"/>
-      <c r="BL31" s="71"/>
-      <c r="BM31" s="71"/>
-      <c r="BN31" s="71"/>
-      <c r="BO31" s="71"/>
-      <c r="BP31" s="71"/>
-      <c r="BQ31" s="71"/>
-      <c r="BR31" s="71"/>
-      <c r="BS31" s="71"/>
-      <c r="BT31" s="71"/>
-      <c r="BU31" s="71"/>
-      <c r="BV31" s="71"/>
-      <c r="BW31" s="71"/>
-      <c r="BX31" s="71"/>
-      <c r="BY31" s="71"/>
-      <c r="BZ31" s="71"/>
-      <c r="CA31" s="71"/>
-      <c r="CB31" s="71"/>
-      <c r="CC31" s="77"/>
-      <c r="CD31" s="78"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="67"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="67"/>
+      <c r="S31" s="67"/>
+      <c r="T31" s="67"/>
+      <c r="U31" s="67"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="67"/>
+      <c r="X31" s="67"/>
+      <c r="Y31" s="67"/>
+      <c r="Z31" s="67"/>
+      <c r="AA31" s="67"/>
+      <c r="AB31" s="67"/>
+      <c r="AC31" s="67"/>
+      <c r="AD31" s="67"/>
+      <c r="AE31" s="67"/>
+      <c r="AF31" s="67"/>
+      <c r="AG31" s="67"/>
+      <c r="AH31" s="67"/>
+      <c r="AI31" s="67"/>
+      <c r="AJ31" s="67"/>
+      <c r="AK31" s="67"/>
+      <c r="AL31" s="67"/>
+      <c r="AM31" s="67"/>
+      <c r="AN31" s="67"/>
+      <c r="AO31" s="67"/>
+      <c r="AP31" s="67"/>
+      <c r="AQ31" s="67"/>
+      <c r="AR31" s="67"/>
+      <c r="AS31" s="67"/>
+      <c r="AT31" s="67"/>
+      <c r="AU31" s="67"/>
+      <c r="AV31" s="67"/>
+      <c r="AW31" s="67"/>
+      <c r="AX31" s="67"/>
+      <c r="AY31" s="67"/>
+      <c r="AZ31" s="67"/>
+      <c r="BA31" s="67"/>
+      <c r="BB31" s="67"/>
+      <c r="BC31" s="67"/>
+      <c r="BD31" s="67"/>
+      <c r="BE31" s="67"/>
+      <c r="BF31" s="67"/>
+      <c r="BG31" s="67"/>
+      <c r="BH31" s="67"/>
+      <c r="BI31" s="67"/>
+      <c r="BJ31" s="67"/>
+      <c r="BK31" s="67"/>
+      <c r="BL31" s="67"/>
+      <c r="BM31" s="67"/>
+      <c r="BN31" s="67"/>
+      <c r="BO31" s="67"/>
+      <c r="BP31" s="67"/>
+      <c r="BQ31" s="67"/>
+      <c r="BR31" s="67"/>
+      <c r="BS31" s="67"/>
+      <c r="BT31" s="67"/>
+      <c r="BU31" s="67"/>
+      <c r="BV31" s="67"/>
+      <c r="BW31" s="67"/>
+      <c r="BX31" s="67"/>
+      <c r="BY31" s="67"/>
+      <c r="BZ31" s="67"/>
+      <c r="CA31" s="67"/>
+      <c r="CB31" s="67"/>
+      <c r="CC31" s="83"/>
+      <c r="CD31" s="84"/>
     </row>
-    <row r="32" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="27" t="s">
         <v>41</v>
       </c>
@@ -4277,7 +4381,7 @@
       <c r="BF32" s="6"/>
       <c r="BG32" s="6"/>
       <c r="BH32" s="6"/>
-      <c r="BI32" s="74"/>
+      <c r="BI32" s="61"/>
       <c r="BJ32" s="6"/>
       <c r="BK32" s="7"/>
       <c r="BL32" s="32"/>
@@ -4297,10 +4401,10 @@
       <c r="BZ32" s="6"/>
       <c r="CA32" s="6"/>
       <c r="CB32" s="57"/>
-      <c r="CC32" s="83">
-        <v>0.1</v>
-      </c>
-      <c r="CD32" s="84"/>
+      <c r="CC32" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="CD32" s="86"/>
     </row>
     <row r="33" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
@@ -4385,10 +4489,12 @@
       <c r="BZ33" s="2"/>
       <c r="CA33" s="2"/>
       <c r="CB33" s="58"/>
-      <c r="CC33" s="85"/>
-      <c r="CD33" s="86"/>
+      <c r="CC33" s="72">
+        <v>0.1</v>
+      </c>
+      <c r="CD33" s="73"/>
     </row>
-    <row r="34" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="27" t="s">
         <v>45</v>
       </c>
@@ -4471,10 +4577,10 @@
       <c r="BZ34" s="2"/>
       <c r="CA34" s="2"/>
       <c r="CB34" s="58"/>
-      <c r="CC34" s="85"/>
-      <c r="CD34" s="86"/>
+      <c r="CC34" s="72"/>
+      <c r="CD34" s="73"/>
     </row>
-    <row r="35" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="27" t="s">
         <v>46</v>
       </c>
@@ -4557,7 +4663,9 @@
       <c r="BZ35" s="2"/>
       <c r="CA35" s="2"/>
       <c r="CB35" s="58"/>
-      <c r="CC35" s="85"/>
+      <c r="CC35" s="85" t="s">
+        <v>50</v>
+      </c>
       <c r="CD35" s="86"/>
     </row>
     <row r="36" spans="1:82" x14ac:dyDescent="0.3">
@@ -4643,8 +4751,10 @@
       <c r="BZ36" s="2"/>
       <c r="CA36" s="2"/>
       <c r="CB36" s="58"/>
-      <c r="CC36" s="85"/>
-      <c r="CD36" s="86"/>
+      <c r="CC36" s="72">
+        <v>0.4</v>
+      </c>
+      <c r="CD36" s="73"/>
     </row>
     <row r="37" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
@@ -4729,8 +4839,8 @@
       <c r="BZ37" s="2"/>
       <c r="CA37" s="2"/>
       <c r="CB37" s="58"/>
-      <c r="CC37" s="85"/>
-      <c r="CD37" s="86"/>
+      <c r="CC37" s="72"/>
+      <c r="CD37" s="73"/>
     </row>
     <row r="38" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="28" t="s">
@@ -4815,96 +4925,96 @@
       <c r="BZ38" s="37"/>
       <c r="CA38" s="37"/>
       <c r="CB38" s="55"/>
-      <c r="CC38" s="87"/>
-      <c r="CD38" s="88"/>
+      <c r="CC38" s="74"/>
+      <c r="CD38" s="75"/>
     </row>
     <row r="39" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="60"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="70"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="71"/>
-      <c r="K39" s="71"/>
-      <c r="L39" s="71"/>
-      <c r="M39" s="71"/>
-      <c r="N39" s="71"/>
-      <c r="O39" s="71"/>
-      <c r="P39" s="71"/>
-      <c r="Q39" s="71"/>
-      <c r="R39" s="71"/>
-      <c r="S39" s="71"/>
-      <c r="T39" s="71"/>
-      <c r="U39" s="71"/>
-      <c r="V39" s="71"/>
-      <c r="W39" s="71"/>
-      <c r="X39" s="71"/>
-      <c r="Y39" s="71"/>
-      <c r="Z39" s="71"/>
-      <c r="AA39" s="71"/>
-      <c r="AB39" s="71"/>
-      <c r="AC39" s="71"/>
-      <c r="AD39" s="71"/>
-      <c r="AE39" s="71"/>
-      <c r="AF39" s="71"/>
-      <c r="AG39" s="71"/>
-      <c r="AH39" s="71"/>
-      <c r="AI39" s="71"/>
-      <c r="AJ39" s="71"/>
-      <c r="AK39" s="71"/>
-      <c r="AL39" s="71"/>
-      <c r="AM39" s="71"/>
-      <c r="AN39" s="71"/>
-      <c r="AO39" s="71"/>
-      <c r="AP39" s="71"/>
-      <c r="AQ39" s="71"/>
-      <c r="AR39" s="71"/>
-      <c r="AS39" s="71"/>
-      <c r="AT39" s="71"/>
-      <c r="AU39" s="71"/>
-      <c r="AV39" s="71"/>
-      <c r="AW39" s="71"/>
-      <c r="AX39" s="71"/>
-      <c r="AY39" s="71"/>
-      <c r="AZ39" s="71"/>
-      <c r="BA39" s="71"/>
-      <c r="BB39" s="71"/>
-      <c r="BC39" s="71"/>
-      <c r="BD39" s="71"/>
-      <c r="BE39" s="71"/>
-      <c r="BF39" s="71"/>
-      <c r="BG39" s="71"/>
-      <c r="BH39" s="71"/>
-      <c r="BI39" s="71"/>
-      <c r="BJ39" s="71"/>
-      <c r="BK39" s="71"/>
-      <c r="BL39" s="71"/>
-      <c r="BM39" s="71"/>
-      <c r="BN39" s="71"/>
-      <c r="BO39" s="71"/>
-      <c r="BP39" s="71"/>
-      <c r="BQ39" s="71"/>
-      <c r="BR39" s="71"/>
-      <c r="BS39" s="71"/>
-      <c r="BT39" s="71"/>
-      <c r="BU39" s="71"/>
-      <c r="BV39" s="71"/>
-      <c r="BW39" s="71"/>
-      <c r="BX39" s="71"/>
-      <c r="BY39" s="71"/>
-      <c r="BZ39" s="71"/>
-      <c r="CA39" s="71"/>
-      <c r="CB39" s="71"/>
-      <c r="CC39" s="77"/>
-      <c r="CD39" s="78"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="67"/>
+      <c r="P39" s="67"/>
+      <c r="Q39" s="67"/>
+      <c r="R39" s="67"/>
+      <c r="S39" s="67"/>
+      <c r="T39" s="67"/>
+      <c r="U39" s="67"/>
+      <c r="V39" s="67"/>
+      <c r="W39" s="67"/>
+      <c r="X39" s="67"/>
+      <c r="Y39" s="67"/>
+      <c r="Z39" s="67"/>
+      <c r="AA39" s="67"/>
+      <c r="AB39" s="67"/>
+      <c r="AC39" s="67"/>
+      <c r="AD39" s="67"/>
+      <c r="AE39" s="67"/>
+      <c r="AF39" s="67"/>
+      <c r="AG39" s="67"/>
+      <c r="AH39" s="67"/>
+      <c r="AI39" s="67"/>
+      <c r="AJ39" s="67"/>
+      <c r="AK39" s="67"/>
+      <c r="AL39" s="67"/>
+      <c r="AM39" s="67"/>
+      <c r="AN39" s="67"/>
+      <c r="AO39" s="67"/>
+      <c r="AP39" s="67"/>
+      <c r="AQ39" s="67"/>
+      <c r="AR39" s="67"/>
+      <c r="AS39" s="67"/>
+      <c r="AT39" s="67"/>
+      <c r="AU39" s="67"/>
+      <c r="AV39" s="67"/>
+      <c r="AW39" s="67"/>
+      <c r="AX39" s="67"/>
+      <c r="AY39" s="67"/>
+      <c r="AZ39" s="67"/>
+      <c r="BA39" s="67"/>
+      <c r="BB39" s="67"/>
+      <c r="BC39" s="67"/>
+      <c r="BD39" s="67"/>
+      <c r="BE39" s="67"/>
+      <c r="BF39" s="67"/>
+      <c r="BG39" s="67"/>
+      <c r="BH39" s="67"/>
+      <c r="BI39" s="67"/>
+      <c r="BJ39" s="67"/>
+      <c r="BK39" s="67"/>
+      <c r="BL39" s="67"/>
+      <c r="BM39" s="67"/>
+      <c r="BN39" s="67"/>
+      <c r="BO39" s="67"/>
+      <c r="BP39" s="67"/>
+      <c r="BQ39" s="67"/>
+      <c r="BR39" s="67"/>
+      <c r="BS39" s="67"/>
+      <c r="BT39" s="67"/>
+      <c r="BU39" s="67"/>
+      <c r="BV39" s="67"/>
+      <c r="BW39" s="67"/>
+      <c r="BX39" s="67"/>
+      <c r="BY39" s="67"/>
+      <c r="BZ39" s="67"/>
+      <c r="CA39" s="67"/>
+      <c r="CB39" s="67"/>
+      <c r="CC39" s="67"/>
+      <c r="CD39" s="76"/>
     </row>
-    <row r="40" spans="1:82" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:82" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
         <v>32</v>
       </c>
@@ -4987,10 +5097,10 @@
       <c r="BZ40" s="6"/>
       <c r="CA40" s="6"/>
       <c r="CB40" s="57"/>
-      <c r="CC40" s="83">
-        <v>0.75</v>
-      </c>
-      <c r="CD40" s="84"/>
+      <c r="CC40" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="CD40" s="86"/>
     </row>
     <row r="41" spans="1:82" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
@@ -5075,8 +5185,10 @@
       <c r="BZ41" s="2"/>
       <c r="CA41" s="2"/>
       <c r="CB41" s="58"/>
-      <c r="CC41" s="85"/>
-      <c r="CD41" s="86"/>
+      <c r="CC41" s="72">
+        <v>0.75</v>
+      </c>
+      <c r="CD41" s="73"/>
     </row>
     <row r="42" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
@@ -5161,10 +5273,10 @@
       <c r="BZ42" s="2"/>
       <c r="CA42" s="2"/>
       <c r="CB42" s="58"/>
-      <c r="CC42" s="85"/>
-      <c r="CD42" s="86"/>
+      <c r="CC42" s="72"/>
+      <c r="CD42" s="73"/>
     </row>
-    <row r="43" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:82" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
         <v>35</v>
       </c>
@@ -5247,10 +5359,10 @@
       <c r="BZ43" s="2"/>
       <c r="CA43" s="2"/>
       <c r="CB43" s="58"/>
-      <c r="CC43" s="85"/>
-      <c r="CD43" s="86"/>
+      <c r="CC43" s="72"/>
+      <c r="CD43" s="73"/>
     </row>
-    <row r="44" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:82" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
         <v>36</v>
       </c>
@@ -5333,7 +5445,9 @@
       <c r="BZ44" s="2"/>
       <c r="CA44" s="2"/>
       <c r="CB44" s="58"/>
-      <c r="CC44" s="85"/>
+      <c r="CC44" s="85" t="s">
+        <v>50</v>
+      </c>
       <c r="CD44" s="86"/>
     </row>
     <row r="45" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -5419,8 +5533,10 @@
       <c r="BZ45" s="2"/>
       <c r="CA45" s="2"/>
       <c r="CB45" s="58"/>
-      <c r="CC45" s="85"/>
-      <c r="CD45" s="86"/>
+      <c r="CC45" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="CD45" s="73"/>
     </row>
     <row r="46" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
@@ -5505,8 +5621,8 @@
       <c r="BZ46" s="2"/>
       <c r="CA46" s="2"/>
       <c r="CB46" s="58"/>
-      <c r="CC46" s="85"/>
-      <c r="CD46" s="86"/>
+      <c r="CC46" s="72"/>
+      <c r="CD46" s="73"/>
     </row>
     <row r="47" spans="1:82" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="51" t="s">
@@ -5591,8 +5707,8 @@
       <c r="BZ47" s="37"/>
       <c r="CA47" s="37"/>
       <c r="CB47" s="55"/>
-      <c r="CC47" s="85"/>
-      <c r="CD47" s="86"/>
+      <c r="CC47" s="72"/>
+      <c r="CD47" s="73"/>
     </row>
     <row r="48" spans="1:82" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
@@ -5677,28 +5793,68 @@
       <c r="BZ48" s="9"/>
       <c r="CA48" s="9"/>
       <c r="CB48" s="59"/>
-      <c r="CC48" s="87"/>
-      <c r="CD48" s="88"/>
+      <c r="CC48" s="74"/>
+      <c r="CD48" s="75"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="31">
+    <mergeCell ref="CC36:CD38"/>
+    <mergeCell ref="CC40:CD40"/>
+    <mergeCell ref="CC44:CD44"/>
+    <mergeCell ref="CC41:CD43"/>
+    <mergeCell ref="CC45:CD48"/>
+    <mergeCell ref="B39:CD39"/>
+    <mergeCell ref="B11:CD11"/>
+    <mergeCell ref="B21:CD21"/>
+    <mergeCell ref="CC12:CD12"/>
+    <mergeCell ref="CC16:CD16"/>
+    <mergeCell ref="CC13:CD15"/>
+    <mergeCell ref="CC17:CD20"/>
+    <mergeCell ref="CC4:CD4"/>
+    <mergeCell ref="CC7:CD7"/>
+    <mergeCell ref="CC5:CD6"/>
+    <mergeCell ref="CC8:CD10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B31:CD31"/>
-    <mergeCell ref="G39:CD39"/>
     <mergeCell ref="CC2:CD2"/>
     <mergeCell ref="CC1:CD1"/>
-    <mergeCell ref="CC40:CD48"/>
-    <mergeCell ref="CC32:CD38"/>
-    <mergeCell ref="CC22:CD30"/>
-    <mergeCell ref="CC12:CD20"/>
-    <mergeCell ref="CC4:CD10"/>
     <mergeCell ref="B3:CD3"/>
-    <mergeCell ref="B11:CD11"/>
-    <mergeCell ref="B21:CD21"/>
     <mergeCell ref="AG1:BK1"/>
     <mergeCell ref="BL1:CB1"/>
     <mergeCell ref="B1:AF1"/>
+    <mergeCell ref="CC22:CD22"/>
+    <mergeCell ref="CC26:CD26"/>
+    <mergeCell ref="CC23:CD25"/>
+    <mergeCell ref="CC27:CD30"/>
+    <mergeCell ref="CC32:CD32"/>
+    <mergeCell ref="CC35:CD35"/>
+    <mergeCell ref="CC33:CD34"/>
   </mergeCells>
+  <conditionalFormatting sqref="CC5:CD6">
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>$CC$5&lt;$CC$8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC13:CD15">
+    <cfRule type="expression" dxfId="7" priority="4">
+      <formula>$CC$13&lt;$CC$17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC23:CD25">
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>$CC$23&lt;$CC$27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC33:CD34">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>$CC$33&lt;$CC$36</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CC41:CD43">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>$CC$41&lt;$CC$45</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>